<commit_message>
Updated the template. Updated the client resource. Added documentation for all methods.
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/publicResources/client/template/Template.xlsx
+++ b/src/main/webapp/WEB-INF/publicResources/client/template/Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapha\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bfcjo\Universiteit\Module 4.2\project\shotmaniacs\src\main\webapp\WEB-INF\publicResources\client\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B4C9B6D-5B8F-49E2-BB41-08B5BA7F20DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC2BBAE-58A6-490E-AC87-5C1491248125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Event Name</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Event Type</t>
   </si>
   <si>
-    <t>Event Start (DD/MM/YYYY HH:MM)</t>
-  </si>
-  <si>
     <t>Duration (hours)</t>
   </si>
   <si>
@@ -62,12 +59,34 @@
   </si>
   <si>
     <t>Booking Type</t>
+  </si>
+  <si>
+    <t>Example Name</t>
+  </si>
+  <si>
+    <t>CLUB_PHOTOGRAPHY</t>
+  </si>
+  <si>
+    <t>Example location</t>
+  </si>
+  <si>
+    <t>Example description</t>
+  </si>
+  <si>
+    <t>PHOTOGRAPHY</t>
+  </si>
+  <si>
+    <t>Event Start
+(YYYY-MM-DD HH:MM)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -161,9 +180,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -176,10 +192,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -412,816 +431,845 @@
   <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.21875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="43.109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.77734375" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="12.6640625" style="5"/>
+    <col min="1" max="1" width="15.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="43.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="12.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="9">
+        <v>36537</v>
+      </c>
+      <c r="D2" s="3">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2</v>
+      </c>
+      <c r="J2" s="3">
+        <v>3</v>
+      </c>
+      <c r="K2" s="3">
+        <v>4</v>
+      </c>
+      <c r="L2" s="3">
+        <v>5</v>
+      </c>
+      <c r="M2" s="3">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="N2" s="4">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="7"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="6"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+      <c r="C4" s="9"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="7"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="6"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="7"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="6"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="7"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="6"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="7"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="6"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="7"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="6"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="7"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="6"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="7"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="6"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="9"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="7"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="6"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="7"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="6"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="7"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="6"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="7"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="6"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="7"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="6"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+      <c r="C16" s="9"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="7"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="6"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="C17" s="9"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="7"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="6"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="9"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="7"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="6"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="C19" s="9"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="7"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="6"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
+      <c r="C20" s="9"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="7"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="6"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="7"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="6"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+      <c r="C22" s="9"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="7"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="6"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+      <c r="C23" s="9"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="7"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="6"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
+      <c r="C24" s="9"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="7"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="6"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
     </row>
-    <row r="25" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
+      <c r="C25" s="9"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="7"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="6"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
+      <c r="C26" s="9"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="7"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="6"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
     </row>
-    <row r="27" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
+      <c r="C27" s="9"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="7"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="6"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
+      <c r="C28" s="9"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="7"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="6"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="C29" s="9"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="7"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="6"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
+      <c r="C30" s="9"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="7"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="6"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
+      <c r="C31" s="9"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="7"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="6"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
+      <c r="C32" s="9"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="7"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="6"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
+      <c r="C33" s="9"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="7"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="6"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
+      <c r="C34" s="9"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="7"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="6"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
+      <c r="C35" s="9"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="7"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="6"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
     </row>
-    <row r="36" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
+      <c r="C36" s="9"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="7"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="6"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
+      <c r="C37" s="9"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="7"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="6"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
+      <c r="C38" s="9"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="7"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="6"/>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
     </row>
-    <row r="39" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
+      <c r="C39" s="9"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="7"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="6"/>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
+      <c r="C40" s="9"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="7"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="6"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
+      <c r="C41" s="9"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="7"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="6"/>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
+      <c r="C42" s="9"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="7"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="6"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
+      <c r="C43" s="9"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="7"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="6"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
+      <c r="C44" s="9"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="7"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="6"/>
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
+      <c r="C45" s="9"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="7"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="6"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
+      <c r="C46" s="9"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="7"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="6"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
+      <c r="C47" s="9"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="7"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="6"/>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
     </row>
-    <row r="48" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
+      <c r="C48" s="9"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="7"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="6"/>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
     </row>
-    <row r="49" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
+      <c r="C49" s="9"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="7"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="6"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
+      <c r="C50" s="9"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="7"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="6"/>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
     </row>
-    <row r="51" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
+      <c r="C51" s="9"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="7"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="6"/>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
@@ -1238,9 +1286,7 @@
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Please enter an integer higher than zero" sqref="D2:D51 H2:N1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{5BC2C62D-0AC2-4A78-88A2-83501B314BA3}">
-      <formula1>44927</formula1>
-    </dataValidation>
+    <dataValidation operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{5BC2C62D-0AC2-4A78-88A2-83501B314BA3}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a valid type from the dropdown" sqref="B2:B1048576" xr:uid="{D8D8BDEA-B09B-45A0-8ABE-DF05F8B63636}">
       <formula1>"CLUB_PHOTOGRAPHY,FESTIVAL,PRODUCT_SHOOT"</formula1>
     </dataValidation>
@@ -1249,5 +1295,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>